<commit_message>
Changed some names in db
</commit_message>
<xml_diff>
--- a/data_backend/resources/domain_data/data_reference_segment.xlsx
+++ b/data_backend/resources/domain_data/data_reference_segment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">reference_seg_id</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">dna_fasta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein_fasta</t>
   </si>
   <si>
     <t xml:space="preserve">PB2</t>
@@ -178,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,10 +189,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,7 +392,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,11 +416,8 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="447.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -435,13 +425,13 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="530.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="479.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -449,14 +439,14 @@
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="417.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -464,14 +454,14 @@
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="328.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -479,14 +469,14 @@
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="353.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -494,13 +484,13 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -508,14 +498,14 @@
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="241.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="210.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
@@ -523,14 +513,14 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="192.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
@@ -538,19 +528,19 @@
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>